<commit_message>
actualización links de interes
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Enlace</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Generador de degradados en CSS</t>
+  </si>
+  <si>
+    <t>https://www.zinefilos.com/</t>
+  </si>
+  <si>
+    <t>Información de peliculas para usar data e imágenes</t>
   </si>
 </sst>
 </file>
@@ -383,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +449,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
@@ -450,6 +464,7 @@
     <hyperlink ref="B5" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modelo de caja y uso de la propiedad display
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Enlace</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Información de peliculas para usar data e imágenes</t>
+  </si>
+  <si>
+    <t>https://git-scm.com/install/</t>
+  </si>
+  <si>
+    <t>Para descargar GIT</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +463,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
@@ -465,6 +479,7 @@
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="B7" r:id="rId5"/>
     <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización de archivo con links de interes
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Enlace</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>Para descargar GIT</t>
+  </si>
+  <si>
+    <t>https://prismic.io/blog/css-hover-effects</t>
+  </si>
+  <si>
+    <t>Algunos ejemplos de efectos en CSS</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/css/css_navbar_horizontal.asp</t>
+  </si>
+  <si>
+    <t>Ejemplo de Menú con CSS</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/css/css3_buttons.asp</t>
+  </si>
+  <si>
+    <t>Ejemplo de botones con css</t>
   </si>
 </sst>
 </file>
@@ -111,9 +129,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -395,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +490,33 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
@@ -480,7 +526,11 @@
     <hyperlink ref="B7" r:id="rId5"/>
     <hyperlink ref="B8" r:id="rId6"/>
     <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización link ejemplos flexbox
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Enlace</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Ejemplo de botones con css</t>
+  </si>
+  <si>
+    <t>https://www.plasmic.app/blog/mastering-css-flexbox-with-plasmic</t>
+  </si>
+  <si>
+    <t>Ejemplos de flexbox (imágenes y código)</t>
   </si>
 </sst>
 </file>
@@ -417,7 +423,7 @@
   <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +521,12 @@
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -529,8 +540,9 @@
     <hyperlink ref="B10" r:id="rId8"/>
     <hyperlink ref="B11" r:id="rId9"/>
     <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización excel links de interes y apuntes uso de consola - git
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Enlace</t>
   </si>
@@ -109,13 +109,19 @@
   </si>
   <si>
     <t>Calculadora de pixeles</t>
+  </si>
+  <si>
+    <t>https://git-scm.com/cheat-sheet</t>
+  </si>
+  <si>
+    <t>Comados Básicos de Git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,14 +133,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,11 +159,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -450,7 +447,7 @@
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,8 +576,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -598,8 +600,9 @@
     <hyperlink ref="B14" r:id="rId12"/>
     <hyperlink ref="B15" r:id="rId13"/>
     <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización links y uso de Markdown
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Enlace</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Página para descargar Node Js</t>
+  </si>
+  <si>
+    <t>https://docs.github.com/es/get-started/writing-on-github/getting-started-with-writing-and-formatting-on-github/basic-writing-and-formatting-syntax</t>
+  </si>
+  <si>
+    <t>Documentación Sintaxis MK archivo readme github</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C19"/>
+  <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +616,14 @@
       </c>
       <c r="C19" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -631,8 +645,9 @@
     <hyperlink ref="B17" r:id="rId15"/>
     <hyperlink ref="B18" r:id="rId16"/>
     <hyperlink ref="B19" r:id="rId17"/>
+    <hyperlink ref="B20" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Avance javascript y se agregó link
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Enlace</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Documentación Sintaxis MK archivo readme github</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/es/docs/Web/JavaScript/Reference/Statements/switch</t>
+  </si>
+  <si>
+    <t>Ejemplos de switch en javascript</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C20"/>
+  <dimension ref="B2:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,6 +630,14 @@
       </c>
       <c r="C20" s="2" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -646,8 +660,9 @@
     <hyperlink ref="B18" r:id="rId16"/>
     <hyperlink ref="B19" r:id="rId17"/>
     <hyperlink ref="B20" r:id="rId18"/>
+    <hyperlink ref="B21" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Métodos de los arrays
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Enlace</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Bucles en javascript</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/es/docs/Web/JavaScript/Reference/Global_Objects/Array</t>
+  </si>
+  <si>
+    <t>Métodos para utilizar en arrays javascript</t>
   </si>
 </sst>
 </file>
@@ -474,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
@@ -652,6 +658,14 @@
       </c>
       <c r="C22" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -676,8 +690,9 @@
     <hyperlink ref="B20" r:id="rId18"/>
     <hyperlink ref="B21" r:id="rId19"/>
     <hyperlink ref="B22" r:id="rId20"/>
+    <hyperlink ref="B23" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Links ejemplos de wallet
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Enlace</t>
   </si>
@@ -151,13 +151,22 @@
   </si>
   <si>
     <t>Métodos para utilizar en arrays javascript</t>
+  </si>
+  <si>
+    <t>https://themeforest.net/search/wallet?srsltid=AfmBOoo8oQOEGuS2iThy6Hil9fR1ffhqVDq8GYZmM_M84hnPVaXUbgiR</t>
+  </si>
+  <si>
+    <t>Inspiración para Wallet</t>
+  </si>
+  <si>
+    <t>https://dribbble.com/tags/my-wallet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +178,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,10 +212,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -480,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C23"/>
+  <dimension ref="B2:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,6 +685,25 @@
       <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -691,8 +728,10 @@
     <hyperlink ref="B21" r:id="rId19"/>
     <hyperlink ref="B22" r:id="rId20"/>
     <hyperlink ref="B23" r:id="rId21"/>
+    <hyperlink ref="B24" r:id="rId22"/>
+    <hyperlink ref="B25" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Otro ejemplo de wallet
</commit_message>
<xml_diff>
--- a/links de interes.xlsx
+++ b/links de interes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Enlace</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>https://dribbble.com/tags/my-wallet</t>
+  </si>
+  <si>
+    <t>https://themeforest.net/item/crypto-admin-responsive-bootstrap-4-admin-html-templates/21604673</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
   <dimension ref="B2:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C25" sqref="C25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,6 +702,14 @@
         <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -730,8 +741,9 @@
     <hyperlink ref="B23" r:id="rId21"/>
     <hyperlink ref="B24" r:id="rId22"/>
     <hyperlink ref="B25" r:id="rId23"/>
+    <hyperlink ref="B26" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>